<commit_message>
REfined user stories for weapons, armors, and build creation generic stories
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexj\Desktop\WORKSPACE\MHW_API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71888436-EE6B-4EA9-9732-C13E5017E2D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8F59F1-87A1-442C-A3E0-543E45847643}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DCC925F4-5354-4FEF-852A-AFB0FB601A22}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DCC925F4-5354-4FEF-852A-AFB0FB601A22}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
   <si>
     <t>ID</t>
   </si>
@@ -85,9 +85,6 @@
     <t>I want to access to a list of existing armors</t>
   </si>
   <si>
-    <t>I want to access to a list of existing decorations</t>
-  </si>
-  <si>
     <t>I want to create my own build</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>I want to access to a list of existing talents</t>
   </si>
   <si>
-    <t>I want to generate a build</t>
-  </si>
-  <si>
     <t>Filtering list with existing armors</t>
   </si>
   <si>
@@ -109,9 +103,6 @@
     <t>Filtering list with existing charms</t>
   </si>
   <si>
-    <t>Filtering list with existing decorations</t>
-  </si>
-  <si>
     <t>Panel for build creation</t>
   </si>
   <si>
@@ -119,6 +110,147 @@
   </si>
   <si>
     <t>Panel for build generation with caracteristics selection</t>
+  </si>
+  <si>
+    <t>US-11</t>
+  </si>
+  <si>
+    <t>US-12</t>
+  </si>
+  <si>
+    <t>The user can browse the complete list of existing armors</t>
+  </si>
+  <si>
+    <t>The user can filter the armor list by type</t>
+  </si>
+  <si>
+    <t>The user can filter the armor list by rarity</t>
+  </si>
+  <si>
+    <t>The user can filter the armor list for specific armorsets</t>
+  </si>
+  <si>
+    <t>Shows a list of all existing armors from the API</t>
+  </si>
+  <si>
+    <t>When clicking on an armor, the user has access to more specific informations about the piece of armor (defense, resistance, etc.)</t>
+  </si>
+  <si>
+    <t>I want to access a list of weapons</t>
+  </si>
+  <si>
+    <t>When entering text in a TextBox the user can filter the list to display  armors containing the text written</t>
+  </si>
+  <si>
+    <t>Filters the list by a selected Armor type in a given list</t>
+  </si>
+  <si>
+    <t>Filters the list by a selected Armorset type in a given list</t>
+  </si>
+  <si>
+    <t>Filters the list by a selected Rarity type in a given list</t>
+  </si>
+  <si>
+    <t>US-13</t>
+  </si>
+  <si>
+    <t>US-14</t>
+  </si>
+  <si>
+    <t>US-15</t>
+  </si>
+  <si>
+    <t>US-16</t>
+  </si>
+  <si>
+    <t>US-17</t>
+  </si>
+  <si>
+    <t>The user has the choice of adding selected armor piece to its current build</t>
+  </si>
+  <si>
+    <t>US-31</t>
+  </si>
+  <si>
+    <t>US-32</t>
+  </si>
+  <si>
+    <t>The user can access its current build</t>
+  </si>
+  <si>
+    <t>Displays every piece constituting the current build</t>
+  </si>
+  <si>
+    <t>The user can save its current build</t>
+  </si>
+  <si>
+    <t>US-33</t>
+  </si>
+  <si>
+    <t>The user can load its current build</t>
+  </si>
+  <si>
+    <t>US-34</t>
+  </si>
+  <si>
+    <t>The user can delete pieces of equipment from the current build</t>
+  </si>
+  <si>
+    <t>On each equipment piece, there is a delete button allowing the user to remove this equipement from the current build.</t>
+  </si>
+  <si>
+    <t>The user can add the currently selected armor piece to its current build</t>
+  </si>
+  <si>
+    <t>The user can select and get details of a specific armor</t>
+  </si>
+  <si>
+    <t>The user is able to persist his current build via a Save button, to use it for later purposes</t>
+  </si>
+  <si>
+    <t>Displays a list of previously saved builds and allows the user to load it</t>
+  </si>
+  <si>
+    <t>I want to access a list of decorations</t>
+  </si>
+  <si>
+    <t>Filtering list with existing weapons</t>
+  </si>
+  <si>
+    <t>US-21</t>
+  </si>
+  <si>
+    <t>US-22</t>
+  </si>
+  <si>
+    <t>US-23</t>
+  </si>
+  <si>
+    <t>US-24</t>
+  </si>
+  <si>
+    <t>US-25</t>
+  </si>
+  <si>
+    <t>US-26</t>
+  </si>
+  <si>
+    <t>US-27</t>
+  </si>
+  <si>
+    <t>The user can browse the complete list of existing weapons</t>
+  </si>
+  <si>
+    <t>Shows a list of all existing weapons from the API</t>
+  </si>
+  <si>
+    <t>The user can filter the armor list by name</t>
+  </si>
+  <si>
+    <t>The user can filter the armor list for sharpness</t>
+  </si>
+  <si>
+    <t>Filters the list by a selected Sharpness attribute</t>
   </si>
 </sst>
 </file>
@@ -134,15 +266,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -150,11 +288,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -165,11 +340,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -178,12 +369,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -202,10 +387,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1BEDE8C4-B8A5-449D-A6A2-A837A2BC10CB}" name="Tableau2" displayName="Tableau2" ref="A1:D7" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:D7" xr:uid="{0D765F28-CC12-4A97-98A6-875964F3505A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1BEDE8C4-B8A5-449D-A6A2-A837A2BC10CB}" name="Tableau2" displayName="Tableau2" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:D9" xr:uid="{0D765F28-CC12-4A97-98A6-875964F3505A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CADF3A40-8056-464C-9026-5D6E5D138A83}" name="ID" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{CADF3A40-8056-464C-9026-5D6E5D138A83}" name="ID" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{28D5B8C8-FBAC-4EE9-AEE6-5BC872CD2512}" name="Context"/>
     <tableColumn id="3" xr3:uid="{387FD88E-8449-4C72-9384-63792D2B584F}" name="Description"/>
     <tableColumn id="4" xr3:uid="{168E329A-8091-4C63-A141-C2C39549A92B}" name="PO"/>
@@ -215,19 +400,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0EC0F617-D470-477E-8C01-ABD2E89C68DD}" name="Tableau1" displayName="Tableau1" ref="A1:C3" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0EC0F617-D470-477E-8C01-ABD2E89C68DD}" name="Tableau1" displayName="Tableau1" ref="A1:C3" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:C3" xr:uid="{2264239A-1F35-4FBE-A312-0F8B79330808}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E7EBC04E-3E87-4EE8-A161-49D47D9CC847}" name="User ID" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{047FBF56-8EAE-428C-9670-19B740A23517}" name="User role" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{C51B5B5C-82A1-444C-A880-080D020ADA32}" name="Context" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{E7EBC04E-3E87-4EE8-A161-49D47D9CC847}" name="User ID" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{047FBF56-8EAE-428C-9670-19B740A23517}" name="User role" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{C51B5B5C-82A1-444C-A880-080D020ADA32}" name="Context" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -523,21 +708,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BD85003-EF2D-4B8D-A07E-08E02CCF0D59}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.109375" customWidth="1"/>
-    <col min="2" max="2" width="81.77734375" customWidth="1"/>
-    <col min="3" max="3" width="46.77734375" customWidth="1"/>
-    <col min="4" max="4" width="32.5546875" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="81.7109375" customWidth="1"/>
+    <col min="3" max="3" width="118.7109375" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +736,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -559,79 +744,299 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="9"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D27" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="D28" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -651,14 +1056,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="2" max="2" width="23.77734375" customWidth="1"/>
-    <col min="3" max="3" width="42.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -669,7 +1074,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="74.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -680,7 +1085,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -691,77 +1096,77 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>

</xml_diff>